<commit_message>
Try one of analyzing the data
</commit_message>
<xml_diff>
--- a/Results/all_logs.xlsx
+++ b/Results/all_logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valeria\Documents\Experimental Design and Analysis\ExperimentalDesign_ClassProject\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0289705B-408E-4A50-860A-7F8D80DEA043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5F3E3D-304C-48CD-94DC-20E0D2C8421A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="3960" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="1110" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J299" sqref="J299"/>
     </sheetView>
   </sheetViews>

</xml_diff>